<commit_message>
added a new entry
</commit_message>
<xml_diff>
--- a/Monthly Expense.xlsx
+++ b/Monthly Expense.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:XFD12"/>
@@ -798,6 +798,28 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>08-08-2024</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Income</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Side Gig</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
New Entry added to the database
</commit_message>
<xml_diff>
--- a/Monthly Expense.xlsx
+++ b/Monthly Expense.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:XFD12"/>
@@ -820,6 +820,28 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>08-07-2024</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Expense</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>SPA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>